<commit_message>
add init -v -h api
</commit_message>
<xml_diff>
--- a/test/TestFile/output/allTest/提取词条EN.xlsx
+++ b/test/TestFile/output/allTest/提取词条EN.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -385,9 +385,170 @@
         <v>EN</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>D:/Git/translate/test/TestFile/test/allTest/html/hello.html</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Hello Title</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Note: &lt;b id="doReboot"&gt;reset&lt;/b&gt; to de ok.</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Note: from &lt;b id="doRebootKiKi"&gt;not the same&lt;/b&gt; no one.</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>this is data-title</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>data lang world</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>random code:</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>copy</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>data lang reBorn</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>重生</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>idone know \n about this</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>generWay</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>random type `` ` code:</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>一键登录</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>免认证</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>idCard</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>phoneNum</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>save</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>save1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>D:/Git/translate/test/TestFile/test/allTest/js/hello.js</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>我们不"一样</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>宏控制词条</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>宏不一样所以肯定被提取</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>没有对应的结束宏，可以被提取</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>符号提(')取验(")证项</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>换行和tab验证：</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>时间组一：</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>类型：</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>系统日志</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Attack 'Log"</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>错误日志</v>
+      </c>
+    </row>
+    <row r="33" xml:space="preserve">
+      <c r="A33" t="str" xml:space="preserve">
+        <v xml:space="preserve">Log 
+ Content</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A33"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>